<commit_message>
Add kenmerktypes for trajecten (optimal, actual speed and time)
</commit_message>
<xml_diff>
--- a/codelist_generator/codelijst.xlsx
+++ b/codelist_generator/codelijst.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\Verkeersmetingen\codelist_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brechtvandevyvere/Documents/OSLOthema-verkeersmetingen/codelist_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9196B83B-589D-44C6-9B18-90B9E25DC5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29540F4E-EA4C-1A40-A83F-0ED35CFC5588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{E3303C72-65BC-460E-B098-279069D7A6E2}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="21100" activeTab="3" xr2:uid="{E3303C72-65BC-460E-B098-279069D7A6E2}"/>
   </bookViews>
   <sheets>
     <sheet name="VkmVoertuigType" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="VkmRijstrookType" sheetId="12" r:id="rId3"/>
     <sheet name="VkmVerkeersKenmerkType" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="203">
   <si>
     <t>Klasse</t>
   </si>
@@ -594,6 +594,60 @@
   </si>
   <si>
     <t>pechstrook</t>
+  </si>
+  <si>
+    <t>actuele_tijd</t>
+  </si>
+  <si>
+    <t>actuele tijd</t>
+  </si>
+  <si>
+    <t>vertraging</t>
+  </si>
+  <si>
+    <t>optimale_tijd</t>
+  </si>
+  <si>
+    <t>de huidige tijd gemeten om een traject af te leggen</t>
+  </si>
+  <si>
+    <t>de optimale tijd om een traject af te leggen</t>
+  </si>
+  <si>
+    <t>de tijd waarin de actuele tijd afwijkt van de optimale tijd om een traject af te leggen</t>
+  </si>
+  <si>
+    <t>optimale tijd</t>
+  </si>
+  <si>
+    <t>trajectgemiddelde snelheid</t>
+  </si>
+  <si>
+    <t>optimale_trajectgemiddelde_snelheid</t>
+  </si>
+  <si>
+    <t>gemiddelde snelheid gemeten over een traject (harmonisch gemiddelde)</t>
+  </si>
+  <si>
+    <t>optimale trajectgemiddelde snelheid</t>
+  </si>
+  <si>
+    <t>actualTt</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>actualKmH</t>
+  </si>
+  <si>
+    <t>optimalKmH</t>
+  </si>
+  <si>
+    <t>optimalTt</t>
+  </si>
+  <si>
+    <t>de optimale gemiddelde snelheid om een traject af te leggen</t>
   </si>
 </sst>
 </file>
@@ -663,9 +717,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -703,7 +757,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -809,7 +863,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -951,7 +1005,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -965,16 +1019,16 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="168.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
-    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="168.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1062,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -1026,7 +1080,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
@@ -1044,7 +1098,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1062,7 +1116,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1080,7 +1134,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1101,15 +1155,15 @@
       <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="120.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1143,7 +1197,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1160,7 +1214,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1177,7 +1231,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1248,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1265,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1228,7 +1282,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1245,7 +1299,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1262,7 +1316,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1279,7 +1333,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1305,21 +1359,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8644C1F-B6A9-4A03-8253-A64EF1B9A9BE}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="173.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="115.75" customWidth="1"/>
-    <col min="5" max="6" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="173.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.6640625" customWidth="1"/>
+    <col min="5" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -1342,7 +1396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1365,7 +1419,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1388,7 +1442,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1411,7 +1465,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1434,7 +1488,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1457,7 +1511,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1480,7 +1534,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1503,7 +1557,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1526,7 +1580,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1549,7 +1603,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1572,7 +1626,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1595,7 +1649,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1618,7 +1672,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1641,7 +1695,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1664,7 +1718,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1687,7 +1741,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1710,7 +1764,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1733,7 +1787,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1756,7 +1810,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1779,7 +1833,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1802,7 +1856,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1825,7 +1879,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1848,7 +1902,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1871,7 +1925,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1894,7 +1948,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1917,7 +1971,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1940,7 +1994,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1971,21 +2025,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4970469-9165-4AAC-9E84-794859EBDEA5}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -2019,7 +2073,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2036,7 +2090,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -2053,7 +2107,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -2070,7 +2124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -2087,7 +2141,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2101,6 +2155,91 @@
         <v>67</v>
       </c>
       <c r="E7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2110,14 +2249,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1fe43d49-4f67-4486-9d33-01c03a937144">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2375,21 +2512,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1fe43d49-4f67-4486-9d33-01c03a937144">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9183F7A-64EE-48EC-89DD-9A50891C3E8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{767BCD5D-D9CA-4F41-921C-9506A605E799}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1fe43d49-4f67-4486-9d33-01c03a937144"/>
-    <ds:schemaRef ds:uri="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2415,9 +2551,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{767BCD5D-D9CA-4F41-921C-9506A605E799}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9183F7A-64EE-48EC-89DD-9A50891C3E8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1fe43d49-4f67-4486-9d33-01c03a937144"/>
+    <ds:schemaRef ds:uri="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>